<commit_message>
Added cambio de Pruebas en archivos csv
</commit_message>
<xml_diff>
--- a/TorneoApp/TorneoApp/Registro.xlsx
+++ b/TorneoApp/TorneoApp/Registro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\Zhang Fei\TorneoAdmin\TorneoApp\TorneoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A654D62-423A-4CE2-BEE5-3F8B0042FC3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6734456E-8293-478E-8A99-E306D35F0FA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -450,11 +450,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -466,11 +466,12 @@
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.85546875" customWidth="1"/>
     <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="20" width="21.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="21" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,14 +508,14 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43636.659293680554</v>
       </c>
@@ -549,14 +550,15 @@
       <c r="L2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>3173694663</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43637.659293634257</v>
       </c>
@@ -591,14 +593,15 @@
       <c r="L3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="2"/>
+      <c r="N3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>3173694664</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43638.659293634257</v>
       </c>
@@ -633,14 +636,15 @@
       <c r="L4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="2"/>
+      <c r="N4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>3173694665</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43639.659293634257</v>
       </c>
@@ -675,10 +679,11 @@
       <c r="L5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="2"/>
+      <c r="N5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>3173694666</v>
       </c>
     </row>

</xml_diff>